<commit_message>
right display of orders
</commit_message>
<xml_diff>
--- a/databases/DefaultCONTRACTS.xlsx
+++ b/databases/DefaultCONTRACTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518172\Documents\GitHub\ATdIT_Gruppe5\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B08254E-01FA-46AB-B084-53ACF250E9A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F7A9EDF-7BCE-41A2-B782-56D07E4B3445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="516" windowWidth="21600" windowHeight="11304" xr2:uid="{4D16F701-1BC3-48A2-907F-84BDB4148723}"/>
+    <workbookView xWindow="720" yWindow="1740" windowWidth="21600" windowHeight="10080" xr2:uid="{4D16F701-1BC3-48A2-907F-84BDB4148723}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>due_date</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>overdue</t>
-  </si>
-  <si>
-    <t>07.03,2020</t>
   </si>
   <si>
     <t>a</t>
@@ -128,12 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,7 +447,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,13 +496,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>300</v>
       </c>
-      <c r="E2" t="s">
-        <v>17</v>
+      <c r="E2">
+        <v>4</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -529,13 +525,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>200</v>
       </c>
-      <c r="E3" s="2">
-        <v>44112</v>
+      <c r="E3">
+        <v>4</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -558,13 +554,13 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>100</v>
       </c>
-      <c r="E4" s="2">
-        <v>44110</v>
+      <c r="E4">
+        <v>4</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -573,10 +569,10 @@
         <v>1</v>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -587,13 +583,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>800</v>
       </c>
-      <c r="E5" s="2">
-        <v>44113</v>
+      <c r="E5">
+        <v>4</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -602,10 +598,10 @@
         <v>1</v>
       </c>
       <c r="H5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
hash & equals von Order & User gekürzt
</commit_message>
<xml_diff>
--- a/databases/DefaultCONTRACTS.xlsx
+++ b/databases/DefaultCONTRACTS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518172\Documents\GitHub\ATdIT_Gruppe5\databases\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>due_date</t>
   </si>
@@ -108,12 +108,16 @@
   </si>
   <si>
     <t>Geliefert</t>
+  </si>
+  <si>
+    <t>Sandstein</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -470,11 +474,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="11.5546875" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="10.109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="16.88671875" collapsed="true"/>
+    <col min="5" max="16384" style="1" width="11.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -638,26 +642,26 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" t="n">
+        <v>5.0</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>800</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>800.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4.0</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="G6" t="n">
+        <v>60000.0</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -665,8 +669,8 @@
       <c r="I6" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="1">
-        <v>1</v>
+      <c r="J6" s="1" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
.delted non code files
</commit_message>
<xml_diff>
--- a/databases/DefaultCONTRACTS.xlsx
+++ b/databases/DefaultCONTRACTS.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>due_date</t>
   </si>
@@ -578,26 +578,26 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="n">
+        <v>3.0</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="D4" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4.0</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="G4" t="n">
+        <v>7500.0</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -605,8 +605,8 @@
       <c r="I4" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="1">
-        <v>1</v>
+      <c r="J4" s="1" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Interface-Segregation funktioniert, anderer kleiner Bug beim Userinsert entdeckt
</commit_message>
<xml_diff>
--- a/databases/DefaultCONTRACTS.xlsx
+++ b/databases/DefaultCONTRACTS.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518172\Documents\GitHub\ATdIT_Gruppe5\databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518185\Documents\GitHub Repositories\HWG Repos\ATdIT_Gruppe5\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7105872E-EB48-4495-A90C-77F738019D74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D5CE63-D7A6-4D02-81A3-A0F60B8C5081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="780" windowWidth="21600" windowHeight="11328" xr2:uid="{4D16F701-1BC3-48A2-907F-84BDB4148723}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4D16F701-1BC3-48A2-907F-84BDB4148723}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>due_date</t>
   </si>
@@ -117,7 +117,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,11 +146,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,303 +476,309 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="10.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="10.109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="16.88671875" collapsed="true"/>
-    <col min="5" max="16384" style="1" width="11.5546875" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5703125" style="3" collapsed="1"/>
+    <col min="7" max="7" width="11.5703125" style="4" collapsed="1"/>
+    <col min="8" max="8" width="11.5703125" style="1" collapsed="1"/>
+    <col min="9" max="9" width="11.5703125" style="3" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" style="4" collapsed="1"/>
+    <col min="11" max="16384" width="11.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>300</v>
       </c>
       <c r="E2">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="5">
         <v>1</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>200</v>
       </c>
       <c r="E3">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="5">
         <v>1</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D4" s="5">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G4" t="n">
-        <v>7500.0</v>
+      <c r="G4" s="5">
+        <v>7500</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="1" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>800</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="5">
         <v>1</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="n">
-        <v>800.0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D6" s="5">
+        <v>800</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="n">
-        <v>60000.0</v>
+      <c r="G6" s="5">
+        <v>60000</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="1" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>800</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="5">
         <v>3</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>800</v>
       </c>
       <c r="E8">
         <v>4</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="5">
         <v>4</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>800</v>
       </c>
       <c r="E9">
         <v>4</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="5">
         <v>5</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Interface-Segregation funktioniert, unnötige imports entfernt, User-Daten können jetzt in die originale Datenbank statt temp_USERS gespeichert werden
</commit_message>
<xml_diff>
--- a/databases/DefaultCONTRACTS.xlsx
+++ b/databases/DefaultCONTRACTS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518185\Documents\GitHub Repositories\HWG Repos\ATdIT_Gruppe5\databases\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
   <si>
     <t>due_date</t>
   </si>
@@ -117,6 +117,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -481,17 +482,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" style="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5703125" style="3" collapsed="1"/>
-    <col min="7" max="7" width="11.5703125" style="4" collapsed="1"/>
-    <col min="8" max="8" width="11.5703125" style="1" collapsed="1"/>
-    <col min="9" max="9" width="11.5703125" style="3" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" style="4" collapsed="1"/>
-    <col min="11" max="16384" width="11.5703125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="10.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="10.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="16.85546875" collapsed="true"/>
+    <col min="5" max="5" style="1" width="11.5703125" collapsed="true"/>
+    <col min="6" max="6" style="3" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" style="4" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" style="1" width="11.5703125" collapsed="true"/>
+    <col min="9" max="9" style="3" width="11.5703125" collapsed="true"/>
+    <col min="10" max="10" style="4" width="11.5703125" collapsed="true"/>
+    <col min="11" max="16384" style="1" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -559,26 +560,26 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
+      <c r="A3" s="5" t="n">
+        <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="5">
-        <v>200</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4.0</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="5">
-        <v>1</v>
+      <c r="G3" s="5" t="n">
+        <v>15000.0</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -586,8 +587,8 @@
       <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="4">
-        <v>1</v>
+      <c r="J3" s="4" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -655,8 +656,8 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>5</v>
+      <c r="A6" s="5" t="n">
+        <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
@@ -664,17 +665,17 @@
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="5">
-        <v>800</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
+      <c r="D6" s="5" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4.0</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="5">
-        <v>60000</v>
+      <c r="G6" s="5" t="n">
+        <v>7500.0</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -682,8 +683,8 @@
       <c r="I6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="4">
-        <v>1</v>
+      <c r="J6" s="4" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>